<commit_message>
changes to slides; updated bib; updated spreadsheet
</commit_message>
<xml_diff>
--- a/Sim-aware vs. Regular SNAP.xlsx
+++ b/Sim-aware vs. Regular SNAP.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32900" yWindow="-500" windowWidth="29600" windowHeight="18520" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Regular SNAP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,17 +84,19 @@
     <t>Error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t># correct reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#  orrect reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -130,10 +132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,7 +181,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$16</c:f>
+              <c:f>Sheet1!$E$5:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -277,7 +279,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$16</c:f>
+              <c:f>Sheet1!$K$5:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -322,7 +324,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$16</c:f>
+              <c:f>Sheet1!$H$5:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -375,7 +377,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$3</c:f>
+              <c:f>Sheet1!$Q$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -387,7 +389,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3</c:f>
+              <c:f>Sheet1!$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -407,7 +409,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$S$3</c:f>
+              <c:f>Sheet1!$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -419,7 +421,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$3</c:f>
+              <c:f>Sheet1!$T$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -431,11 +433,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="472436600"/>
-        <c:axId val="472433384"/>
+        <c:axId val="513675608"/>
+        <c:axId val="513669352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472436600"/>
+        <c:axId val="513675608"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -464,12 +466,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472433384"/>
+        <c:crossAx val="513669352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472433384"/>
+        <c:axId val="513669352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +497,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472436600"/>
+        <c:crossAx val="513675608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -550,7 +552,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$16</c:f>
+              <c:f>Sheet1!$E$5:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -648,7 +650,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$16</c:f>
+              <c:f>Sheet1!$K$5:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -693,7 +695,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$16</c:f>
+              <c:f>Sheet1!$G$5:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -746,7 +748,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$3</c:f>
+              <c:f>Sheet1!$Q$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -758,7 +760,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3</c:f>
+              <c:f>Sheet1!$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -778,23 +780,23 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet1!$W$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1078.748651564186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$S$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1078.748651564186</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$P$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
                   <c:v>94.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -802,11 +804,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="488823128"/>
-        <c:axId val="488833864"/>
+        <c:axId val="522224392"/>
+        <c:axId val="522246312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="488823128"/>
+        <c:axId val="522224392"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -835,12 +837,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="488833864"/>
+        <c:crossAx val="522246312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="488833864"/>
+        <c:axId val="522246312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +868,374 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="488823128"/>
+        <c:crossAx val="522224392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># Correct Reads vs. Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SNAP</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>53.82131324004305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.2990834539315</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.40988179041041</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.61668641056016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.68800497203232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.08408109006314</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.23788934968675</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.76876421531463</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>102.1033285685113</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>107.2501072501072</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>111.9068934646374</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116.918040453642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>918694.99341</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>918920.04022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>919147.02848</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>919274.0421999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>919386.99345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>919601.95998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>919702.9611</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>919812.9774600001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>919918.028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>919927.964</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>920029.9803899999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>920135.95408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sim-SNAP</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>224.618149146451</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>235.4048964218456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>244.6183953033268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252.7805864509606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260.5523710265763</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.0341673392521</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>277.0083102493075</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>291.4602156805596</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>295.3337271116362</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>303.4901365705614</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>310.1736972704715</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>321.7503217503217</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>911287.97084</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>911587.96688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>911787.96424</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>911987.9616</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>912187.95896</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>912287.95764</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>912488.95875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>912588.9575400001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>912689.9603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>912789.9592</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>912889.9581</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>912989.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BWA</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>925.925925925926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>907636.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Novoalign</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1078.748651564186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>945810.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="539756648"/>
+        <c:axId val="539765672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="539756648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539765672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="539765672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># Correct Reads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539756648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -895,7 +1264,7 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -919,13 +1288,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -942,6 +1311,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1270,42 +1669,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:S16"/>
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="1" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1313,49 +1717,61 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
         <v>13</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>91.78</v>
       </c>
@@ -1363,53 +1779,69 @@
         <v>3.236E-2</v>
       </c>
       <c r="C3">
+        <f>1000000*A3/100*(1-B3/100)</f>
+        <v>917502.99991999997</v>
+      </c>
+      <c r="D3">
         <v>339</v>
       </c>
-      <c r="D3">
-        <f>1000000/C3</f>
+      <c r="E3">
+        <f>1000000/D3</f>
         <v>2949.8525073746314</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>91.03</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2.0899999999999998E-3</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <f>1000000*G3/100*(1-H3/100)</f>
+        <v>910280.97473000002</v>
+      </c>
+      <c r="J3">
         <v>236</v>
       </c>
-      <c r="I3">
-        <f>1000000/H3</f>
+      <c r="K3">
+        <f>1000000/J3</f>
         <v>4237.2881355932204</v>
       </c>
-      <c r="K3" s="3">
+      <c r="M3" s="2">
         <v>90.8</v>
       </c>
-      <c r="L3" s="3">
+      <c r="N3" s="2">
         <v>0.04</v>
       </c>
-      <c r="M3">
+      <c r="O3" s="2">
+        <f>1000000*M3/100*(1-N3/100)</f>
+        <v>907636.8</v>
+      </c>
+      <c r="P3">
         <v>1080</v>
       </c>
-      <c r="N3">
-        <f>1000000/M3</f>
+      <c r="Q3">
+        <f>1000000/P3</f>
         <v>925.92592592592598</v>
       </c>
-      <c r="P3" s="3">
+      <c r="S3" s="2">
         <v>94.6</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="T3" s="2">
         <v>0.02</v>
       </c>
-      <c r="R3">
+      <c r="U3" s="2">
+        <f>1000000*S3/100*(1-T3/100)</f>
+        <v>945810.8</v>
+      </c>
+      <c r="V3">
         <v>927</v>
       </c>
-      <c r="S3">
-        <f>1000000/R3</f>
+      <c r="W3">
+        <f>1000000/V3</f>
         <v>1078.7486515641856</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>91.85</v>
       </c>
@@ -1417,27 +1849,35 @@
         <v>2.5700000000000001E-2</v>
       </c>
       <c r="C4">
+        <f t="shared" ref="C4:C16" si="0">1000000*A4/100*(1-B4/100)</f>
+        <v>918263.94550000003</v>
+      </c>
+      <c r="D4">
         <v>15662</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D16" si="0">1000000/C4</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E16" si="1">1000000/D4</f>
         <v>63.848806027327292</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>91.08</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.32E-3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <f t="shared" ref="I4:I16" si="2">1000000*G4/100*(1-H4/100)</f>
+        <v>910787.97743999993</v>
+      </c>
+      <c r="J4">
         <v>1987</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I16" si="1">1000000/H4</f>
+      <c r="K4">
+        <f t="shared" ref="K4:K16" si="3">1000000/J4</f>
         <v>503.27126321087064</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>91.89</v>
       </c>
@@ -1445,27 +1885,35 @@
         <v>2.231E-2</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>918694.99341</v>
+      </c>
+      <c r="D5">
         <v>18580</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="E5">
+        <f t="shared" si="1"/>
         <v>53.821313240043054</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>91.13</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.32E-3</v>
       </c>
-      <c r="H5">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>911287.97083999997</v>
+      </c>
+      <c r="J5">
         <v>4452</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
+      <c r="K5">
+        <f t="shared" si="3"/>
         <v>224.61814914645103</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>91.91</v>
       </c>
@@ -1473,27 +1921,35 @@
         <v>1.958E-2</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>918920.04022000008</v>
+      </c>
+      <c r="D6">
         <v>16584</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="E6">
+        <f t="shared" si="1"/>
         <v>60.299083453931502</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>91.16</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.32E-3</v>
       </c>
-      <c r="H6">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>911587.96687999996</v>
+      </c>
+      <c r="J6">
         <v>4248</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
+      <c r="K6">
+        <f t="shared" si="3"/>
         <v>235.40489642184556</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>91.93</v>
       </c>
@@ -1501,27 +1957,35 @@
         <v>1.6639999999999999E-2</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>919147.02847999998</v>
+      </c>
+      <c r="D7">
         <v>15058</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>66.40988179041041</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>91.18</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.32E-3</v>
       </c>
-      <c r="H7">
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>911787.96424</v>
+      </c>
+      <c r="J7">
         <v>4088</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
+      <c r="K7">
+        <f t="shared" si="3"/>
         <v>244.61839530332682</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>91.94</v>
       </c>
@@ -1529,27 +1993,35 @@
         <v>1.37E-2</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>919274.04219999991</v>
+      </c>
+      <c r="D8">
         <v>11818</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
+      <c r="E8">
+        <f t="shared" si="1"/>
         <v>84.616686410560163</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>91.2</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.32E-3</v>
       </c>
-      <c r="H8">
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>911987.96159999992</v>
+      </c>
+      <c r="J8">
         <v>3956</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
+      <c r="K8">
+        <f t="shared" si="3"/>
         <v>252.78058645096056</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>91.95</v>
       </c>
@@ -1557,27 +2029,35 @@
         <v>1.2290000000000001E-2</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>919386.99344999995</v>
+      </c>
+      <c r="D9">
         <v>12872</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
+      <c r="E9">
+        <f t="shared" si="1"/>
         <v>77.688004972032317</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>91.22</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1.32E-3</v>
       </c>
-      <c r="H9">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>912187.95895999996</v>
+      </c>
+      <c r="J9">
         <v>3838</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
+      <c r="K9">
+        <f t="shared" si="3"/>
         <v>260.55237102657634</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:23">
       <c r="A10">
         <v>91.97</v>
       </c>
@@ -1585,27 +2065,35 @@
         <v>1.0659999999999999E-2</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>919601.95998000004</v>
+      </c>
+      <c r="D10">
         <v>12036</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>83.084081090063137</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>91.23</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1.32E-3</v>
       </c>
-      <c r="H10">
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>912287.95763999992</v>
+      </c>
+      <c r="J10">
         <v>3717</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
+      <c r="K10">
+        <f t="shared" si="3"/>
         <v>269.03416733925206</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:23">
       <c r="A11">
         <v>91.98</v>
       </c>
@@ -1613,27 +2101,35 @@
         <v>1.055E-2</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>919702.96110000007</v>
+      </c>
+      <c r="D11">
         <v>11333</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
+      <c r="E11">
+        <f t="shared" si="1"/>
         <v>88.237889349686753</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>91.25</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="H11">
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>912488.95874999999</v>
+      </c>
+      <c r="J11">
         <v>3610</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
+      <c r="K11">
+        <f t="shared" si="3"/>
         <v>277.0083102493075</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:23">
       <c r="A12">
         <v>91.99</v>
       </c>
@@ -1641,27 +2137,35 @@
         <v>9.4599999999999997E-3</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
+        <v>919812.97746000008</v>
+      </c>
+      <c r="D12">
         <v>10552</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
+      <c r="E12">
+        <f t="shared" si="1"/>
         <v>94.768764215314633</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>91.26</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1.2099999999999999E-3</v>
       </c>
-      <c r="H12">
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>912588.95754000009</v>
+      </c>
+      <c r="J12">
         <v>3431</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
+      <c r="K12">
+        <f t="shared" si="3"/>
         <v>291.4602156805596</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:23">
       <c r="A13">
         <v>92</v>
       </c>
@@ -1669,27 +2173,35 @@
         <v>8.9099999999999995E-3</v>
       </c>
       <c r="C13">
+        <f t="shared" si="0"/>
+        <v>919918.02800000005</v>
+      </c>
+      <c r="D13">
         <v>9794</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+      <c r="E13">
+        <f t="shared" si="1"/>
         <v>102.10332856851133</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>91.27</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>912689.96030000004</v>
+      </c>
+      <c r="J13">
         <v>3386</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
+      <c r="K13">
+        <f t="shared" si="3"/>
         <v>295.33372711163616</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:23">
       <c r="A14">
         <v>92</v>
       </c>
@@ -1697,27 +2209,35 @@
         <v>7.8300000000000002E-3</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
+        <v>919927.96400000004</v>
+      </c>
+      <c r="D14">
         <v>9324</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+      <c r="E14">
+        <f t="shared" si="1"/>
         <v>107.25010725010725</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>91.28</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="H14">
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>912789.95920000004</v>
+      </c>
+      <c r="J14">
         <v>3295</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
+      <c r="K14">
+        <f t="shared" si="3"/>
         <v>303.49013657056145</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:23">
       <c r="A15">
         <v>92.01</v>
       </c>
@@ -1725,27 +2245,35 @@
         <v>7.6099999999999996E-3</v>
       </c>
       <c r="C15">
+        <f t="shared" si="0"/>
+        <v>920029.98038999992</v>
+      </c>
+      <c r="D15">
         <v>8936</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+      <c r="E15">
+        <f t="shared" si="1"/>
         <v>111.90689346463742</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>91.29</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="H15">
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>912889.95810000005</v>
+      </c>
+      <c r="J15">
         <v>3224</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
+      <c r="K15">
+        <f t="shared" si="3"/>
         <v>310.17369727047145</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:23">
       <c r="A16">
         <v>92.02</v>
       </c>
@@ -1753,36 +2281,43 @@
         <v>6.96E-3</v>
       </c>
       <c r="C16">
+        <f t="shared" si="0"/>
+        <v>920135.95408000005</v>
+      </c>
+      <c r="D16">
         <v>8553</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
+      <c r="E16">
+        <f t="shared" si="1"/>
         <v>116.91804045364199</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>91.3</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>912989.04399999999</v>
+      </c>
+      <c r="J16">
         <v>3108</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
+      <c r="K16">
+        <f t="shared" si="3"/>
         <v>321.75032175032175</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>